<commit_message>
Sample wkbk mods after talking with M. Fraas
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/valid_print_workbook_sketch.xlsx
+++ b/openn/tests/data/sheets/valid_print_workbook_sketch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeryr/code/GIT/openn/openn/tests/data/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6086772B-B8D7-4A49-9AB4-7870D19455B2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{07A74113-B5F9-934D-9AFA-E743859F600D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19960" windowHeight="22580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -2160,7 +2160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4070" uniqueCount="3795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4074" uniqueCount="3798">
   <si>
     <t>1r</t>
   </si>
@@ -13545,6 +13545,15 @@
   </si>
   <si>
     <t>Volume information</t>
+  </si>
+  <si>
+    <t>fileDesc/publicationStmt/publisher</t>
+  </si>
+  <si>
+    <t>Metadata Publisher</t>
+  </si>
+  <si>
+    <t>Kislak Centrer, U. Miami</t>
   </si>
 </sst>
 </file>
@@ -13698,7 +13707,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -13795,6 +13804,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14115,11 +14130,11 @@
   </sheetPr>
   <dimension ref="A1:Z955"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -14583,10 +14598,18 @@
       <c r="Z13" s="15"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="16"/>
+      <c r="A14" s="44" t="s">
+        <v>3795</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>3796</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>3797</v>
+      </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -16058,7 +16081,7 @@
     <row r="955" ht="15.75" customHeight="1"/>
   </sheetData>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="TEI Publication date" prompt="The year this metadata document will be marked a published; e.g., 2018, 2019, etc. _x000a__x000a_NOT the year of the book's publication." sqref="B13:B14 B16:B23" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="TEI Publication date" prompt="The year this metadata document will be marked a published; e.g., 2018, 2019, etc. _x000a__x000a_NOT the year of the book's publication." sqref="B16:B23 B13" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Physical volume title" prompt="A name for the whole volume. This name will appear in the title of the TEI document. If the title of the volume is &quot;The Adventures of Huckleberry Finn&quot; and the call number is PS1305 .R3, the TEI title will be &quot;Description of PS1305 .R3, The Adventures of " sqref="B25" xr:uid="{2F93273A-EFEE-8047-BECB-5FBB0761E1A2}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16071,7 +16094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4409782F-2D3D-7644-911B-01BA111EB3B8}">
   <dimension ref="A1:Z968"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:A29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
WIP: working on flexbile sheet handling
</commit_message>
<xml_diff>
--- a/openn/tests/data/sheets/valid_print_workbook_sketch.xlsx
+++ b/openn/tests/data/sheets/valid_print_workbook_sketch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeryr/code/GIT/openn/openn/tests/data/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{62754AE1-ACAC-4246-BFDF-24E59456AF4A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{45CED583-D2FD-D941-BCF6-A1C5B2B894EA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38260" windowHeight="20420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38260" windowHeight="20420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -2207,7 +2207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4074" uniqueCount="3798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4074" uniqueCount="3802">
   <si>
     <t>1r</t>
   </si>
@@ -13601,6 +13601,18 @@
   </si>
   <si>
     <t>Kislak Centrer, U. Miami</t>
+  </si>
+  <si>
+    <t>ISTC2</t>
+  </si>
+  <si>
+    <t>https://data.cerl.org/istc/ic00759000_2</t>
+  </si>
+  <si>
+    <t>Epistola de insulis nuper inventis 2</t>
+  </si>
+  <si>
+    <t>3rd. Ed. 2</t>
   </si>
 </sst>
 </file>
@@ -13754,7 +13766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -13857,6 +13869,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -16141,7 +16154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4409782F-2D3D-7644-911B-01BA111EB3B8}">
   <dimension ref="A1:Z968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:A29"/>
     </sheetView>
   </sheetViews>
@@ -18542,8 +18555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB615017-EA21-B54B-AA1C-E116925D81D5}">
   <dimension ref="A1:Z968"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15"/>
@@ -18780,8 +18793,8 @@
       <c r="C7" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="36" t="s">
-        <v>3745</v>
+      <c r="D7" s="46" t="s">
+        <v>3799</v>
       </c>
       <c r="E7" s="24"/>
       <c r="F7" s="16"/>
@@ -18817,7 +18830,7 @@
         <v>350</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>3770</v>
+        <v>3798</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="16"/>
@@ -18881,7 +18894,7 @@
         <v>65</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>3730</v>
+        <v>3800</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
@@ -18917,7 +18930,7 @@
         <v>230</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>3789</v>
+        <v>3801</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
@@ -20933,9 +20946,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D41" r:id="rId1" xr:uid="{0FBDD0F3-28FE-404A-B4E8-F788FA18BE1A}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{3CE4825C-399E-944F-B3CF-80CA8CB80CE2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>